<commit_message>
add user equation code
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -492,19 +492,19 @@
         <v>0.1</v>
       </c>
       <c r="B3" t="n">
-        <v>3.292383755317094e-13</v>
+        <v>0.001</v>
       </c>
       <c r="C3" t="n">
-        <v>-3.23452943441852e-13</v>
+        <v>-0.0009824278318694955</v>
       </c>
       <c r="D3" t="n">
-        <v>5.785432089857433e-15</v>
+        <v>1.757216813050468e-05</v>
       </c>
       <c r="E3" t="n">
-        <v>-3.27002683339768e-15</v>
+        <v>-9.932095030285254e-06</v>
       </c>
       <c r="F3" t="n">
-        <v>-2.515405256459754e-15</v>
+        <v>-7.640073100219423e-06</v>
       </c>
     </row>
     <row r="4">
@@ -512,19 +512,19 @@
         <v>0.2</v>
       </c>
       <c r="B4" t="n">
-        <v>6.584767510634188e-13</v>
+        <v>0.008000000000000002</v>
       </c>
       <c r="C4" t="n">
-        <v>-6.418820071070406e-13</v>
+        <v>-0.007844163559570896</v>
       </c>
       <c r="D4" t="n">
-        <v>1.659474395637818e-14</v>
+        <v>0.0001558364404291058</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.536136294128816e-15</v>
+        <v>-7.944486195533348e-05</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.005860766224937e-14</v>
+        <v>-7.63915784737723e-05</v>
       </c>
     </row>
     <row r="5">
@@ -532,19 +532,19 @@
         <v>0.3</v>
       </c>
       <c r="B5" t="n">
-        <v>2.495003886931552e-12</v>
+        <v>0.02700000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>-2.436317421798747e-12</v>
+        <v>-0.02638891150794136</v>
       </c>
       <c r="D5" t="n">
-        <v>5.868646513280515e-14</v>
+        <v>0.0006110884920586503</v>
       </c>
       <c r="E5" t="n">
-        <v>-2.464351235547552e-14</v>
+        <v>-0.0002676787503065252</v>
       </c>
       <c r="F5" t="n">
-        <v>-3.404295277732962e-14</v>
+        <v>-0.0003434097417521251</v>
       </c>
     </row>
     <row r="6">
@@ -552,19 +552,19 @@
         <v>0.4</v>
       </c>
       <c r="B6" t="n">
-        <v>1.316953502126838e-12</v>
+        <v>0.06400000000000002</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.241210908568575e-12</v>
+        <v>-0.06233185230461617</v>
       </c>
       <c r="D6" t="n">
-        <v>7.574259355826263e-14</v>
+        <v>0.001668147695383843</v>
       </c>
       <c r="E6" t="n">
-        <v>-1.285479159119016e-14</v>
+        <v>-0.0006323828649629163</v>
       </c>
       <c r="F6" t="n">
-        <v>-6.288780196707247e-14</v>
+        <v>-0.001035764830420926</v>
       </c>
     </row>
     <row r="7">
@@ -572,19 +572,19 @@
         <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>1.389031173221228e-13</v>
+        <v>0.125</v>
       </c>
       <c r="C7" t="n">
-        <v>-6.556209017885229e-14</v>
+        <v>-0.1212996897185551</v>
       </c>
       <c r="D7" t="n">
-        <v>7.334102714327047e-14</v>
+        <v>0.003700310281444933</v>
       </c>
       <c r="E7" t="n">
-        <v>-3.19304842550972e-16</v>
+        <v>-0.001231098357116649</v>
       </c>
       <c r="F7" t="n">
-        <v>-7.30217223007195e-14</v>
+        <v>-0.002469211924328284</v>
       </c>
     </row>
     <row r="8">
@@ -592,19 +592,19 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B8" t="n">
-        <v>4.990007773863104e-12</v>
+        <v>0.2160000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>-4.829584261482272e-12</v>
+        <v>-0.2088336968083816</v>
       </c>
       <c r="D8" t="n">
-        <v>1.604235123808322e-13</v>
+        <v>0.007166303191618545</v>
       </c>
       <c r="E8" t="n">
-        <v>-4.926218359199808e-14</v>
+        <v>-0.002119617517548127</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.111613287888342e-13</v>
+        <v>-0.005046685674070419</v>
       </c>
     </row>
     <row r="9">
@@ -612,19 +612,19 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="B9" t="n">
-        <v>1.802239041943157e-12</v>
+        <v>0.3430000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.623823836263292e-12</v>
+        <v>-0.3303889817942656</v>
       </c>
       <c r="D9" t="n">
-        <v>1.78415205679866e-13</v>
+        <v>0.01261101820573446</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.659472015927967e-14</v>
+        <v>-0.003353919466789186</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.618204855205863e-13</v>
+        <v>-0.009257098738945273</v>
       </c>
     </row>
     <row r="10">
@@ -632,19 +632,19 @@
         <v>0.8</v>
       </c>
       <c r="B10" t="n">
-        <v>2.633907004253675e-12</v>
+        <v>0.5120000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.416729475201976e-12</v>
+        <v>-0.4913381910815169</v>
       </c>
       <c r="D10" t="n">
-        <v>2.17177529051699e-13</v>
+        <v>0.02066180891848324</v>
       </c>
       <c r="E10" t="n">
-        <v>-2.40736680135508e-14</v>
+        <v>-0.004987914681134856</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.931038610381482e-13</v>
+        <v>-0.01567389423734838</v>
       </c>
     </row>
     <row r="11">
@@ -652,19 +652,19 @@
         <v>0.9</v>
       </c>
       <c r="B11" t="n">
-        <v>-5.538617276662718e-13</v>
+        <v>0.7290000000000001</v>
       </c>
       <c r="C11" t="n">
-        <v>7.536848200591081e-13</v>
+        <v>-0.6969700852614578</v>
       </c>
       <c r="D11" t="n">
-        <v>1.998230923928362e-13</v>
+        <v>0.03202991473854228</v>
       </c>
       <c r="E11" t="n">
-        <v>6.668985761937585e-15</v>
+        <v>-0.00707604868279009</v>
       </c>
       <c r="F11" t="n">
-        <v>-2.064920781547738e-13</v>
+        <v>-0.02495386605575219</v>
       </c>
     </row>
     <row r="12">
@@ -672,19 +672,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>2.778062346442455e-13</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>-7.778114031168949e-14</v>
+        <v>-0.9524937969742547</v>
       </c>
       <c r="D12" t="n">
-        <v>2.00025094332556e-13</v>
+        <v>0.04750620302574527</v>
       </c>
       <c r="E12" t="n">
-        <v>7.556926986719469e-16</v>
+        <v>-0.009670430164435181</v>
       </c>
       <c r="F12" t="n">
-        <v>-2.00780787031228e-13</v>
+        <v>-0.03783577286131009</v>
       </c>
     </row>
   </sheetData>
@@ -747,13 +747,13 @@
         <v>0.1</v>
       </c>
       <c r="B3" t="n">
-        <v>-3.292383755317094e-13</v>
+        <v>-0.001</v>
       </c>
       <c r="C3" t="n">
-        <v>-5.785432089857433e-15</v>
+        <v>-1.757216813050468e-05</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.515405256459754e-15</v>
+        <v>-7.640073100219423e-06</v>
       </c>
     </row>
     <row r="4">
@@ -761,13 +761,13 @@
         <v>0.2</v>
       </c>
       <c r="B4" t="n">
-        <v>-6.584767510634188e-13</v>
+        <v>-0.008000000000000002</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.659474395637818e-14</v>
+        <v>-0.0001558364404291058</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.005860766224937e-14</v>
+        <v>-7.63915784737723e-05</v>
       </c>
     </row>
     <row r="5">
@@ -775,13 +775,13 @@
         <v>0.3</v>
       </c>
       <c r="B5" t="n">
-        <v>-2.495003886931552e-12</v>
+        <v>-0.02700000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>-5.868646513280515e-14</v>
+        <v>-0.0006110884920586503</v>
       </c>
       <c r="D5" t="n">
-        <v>-3.404295277732962e-14</v>
+        <v>-0.0003434097417521251</v>
       </c>
     </row>
     <row r="6">
@@ -789,13 +789,13 @@
         <v>0.4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.316953502126838e-12</v>
+        <v>-0.06400000000000002</v>
       </c>
       <c r="C6" t="n">
-        <v>-7.574259355826263e-14</v>
+        <v>-0.001668147695383843</v>
       </c>
       <c r="D6" t="n">
-        <v>-6.288780196707247e-14</v>
+        <v>-0.001035764830420926</v>
       </c>
     </row>
     <row r="7">
@@ -803,13 +803,13 @@
         <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.389031173221228e-13</v>
+        <v>-0.125</v>
       </c>
       <c r="C7" t="n">
-        <v>-7.334102714327047e-14</v>
+        <v>-0.003700310281444933</v>
       </c>
       <c r="D7" t="n">
-        <v>-7.30217223007195e-14</v>
+        <v>-0.002469211924328284</v>
       </c>
     </row>
     <row r="8">
@@ -817,13 +817,13 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B8" t="n">
-        <v>-4.990007773863104e-12</v>
+        <v>-0.2160000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.604235123808322e-13</v>
+        <v>-0.007166303191618545</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.111613287888342e-13</v>
+        <v>-0.005046685674070419</v>
       </c>
     </row>
     <row r="9">
@@ -831,13 +831,13 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.802239041943157e-12</v>
+        <v>-0.3430000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.78415205679866e-13</v>
+        <v>-0.01261101820573446</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.618204855205863e-13</v>
+        <v>-0.009257098738945273</v>
       </c>
     </row>
     <row r="10">
@@ -845,13 +845,13 @@
         <v>0.8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.633907004253675e-12</v>
+        <v>-0.5120000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>-2.17177529051699e-13</v>
+        <v>-0.02066180891848324</v>
       </c>
       <c r="D10" t="n">
-        <v>-1.931038610381482e-13</v>
+        <v>-0.01567389423734838</v>
       </c>
     </row>
     <row r="11">
@@ -859,13 +859,13 @@
         <v>0.9</v>
       </c>
       <c r="B11" t="n">
-        <v>5.538617276662718e-13</v>
+        <v>-0.7290000000000001</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.998230923928362e-13</v>
+        <v>-0.03202991473854228</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.064920781547738e-13</v>
+        <v>-0.02495386605575219</v>
       </c>
     </row>
     <row r="12">
@@ -873,13 +873,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.778062346442455e-13</v>
+        <v>-1</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.00025094332556e-13</v>
+        <v>-0.04750620302574527</v>
       </c>
       <c r="D12" t="n">
-        <v>-2.00780787031228e-13</v>
+        <v>-0.03783577286131009</v>
       </c>
     </row>
   </sheetData>
@@ -958,19 +958,19 @@
         <v>0.1</v>
       </c>
       <c r="B3" t="n">
-        <v>-2.526976120639468e-14</v>
+        <v>-7.675217436480435e-05</v>
       </c>
       <c r="C3" t="n">
-        <v>-2.526976120639468e-14</v>
+        <v>-7.675217436480433e-05</v>
       </c>
       <c r="D3" t="n">
-        <v>1.157086417971487e-16</v>
+        <v>3.514433626100935e-07</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.515405256459754e-14</v>
+        <v>-7.640073100219427e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>-2.515405256459754e-14</v>
+        <v>-7.640073100219423e-05</v>
       </c>
     </row>
     <row r="4">
@@ -978,19 +978,19 @@
         <v>0.2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.006865542180269e-13</v>
+        <v>-0.000766329626821085</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.006865542180269e-13</v>
+        <v>-0.0007663296268210849</v>
       </c>
       <c r="D4" t="n">
-        <v>1.004775955332663e-16</v>
+        <v>2.413842083361928e-06</v>
       </c>
       <c r="E4" t="n">
-        <v>-1.005860766224937e-13</v>
+        <v>-0.0007639157847377231</v>
       </c>
       <c r="F4" t="n">
-        <v>-1.005860766224937e-13</v>
+        <v>-0.0007639157847377229</v>
       </c>
     </row>
     <row r="5">
@@ -998,19 +998,19 @@
         <v>0.3</v>
       </c>
       <c r="B5" t="n">
-        <v>-3.411708846012916e-13</v>
+        <v>-0.00344078861647048</v>
       </c>
       <c r="C5" t="n">
-        <v>-3.411708846012916e-13</v>
+        <v>-0.00344078861647048</v>
       </c>
       <c r="D5" t="n">
-        <v>7.41356827995273e-16</v>
+        <v>6.691198949228962e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>-3.404295277732963e-13</v>
+        <v>-0.003434097417521252</v>
       </c>
       <c r="F5" t="n">
-        <v>-3.404295277732962e-13</v>
+        <v>-0.003434097417521252</v>
       </c>
     </row>
     <row r="6">
@@ -1018,19 +1018,19 @@
         <v>0.4</v>
       </c>
       <c r="B6" t="n">
-        <v>-6.284777854112386e-13</v>
+        <v>-0.01037209828932654</v>
       </c>
       <c r="C6" t="n">
-        <v>-6.284777854112385e-13</v>
+        <v>-0.01037209828932654</v>
       </c>
       <c r="D6" t="n">
-        <v>-4.002342594861232e-16</v>
+        <v>1.444998511727488e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>-6.288780196707246e-13</v>
+        <v>-0.01035764830420926</v>
       </c>
       <c r="F6" t="n">
-        <v>-6.288780196707246e-13</v>
+        <v>-0.01035764830420926</v>
       </c>
     </row>
     <row r="7">
@@ -1038,19 +1038,19 @@
         <v>0.5</v>
       </c>
       <c r="B7" t="n">
-        <v>-7.305694259383813e-13</v>
+        <v>-0.02471831250988679</v>
       </c>
       <c r="C7" t="n">
-        <v>-7.305694259383812e-13</v>
+        <v>-0.02471831250988679</v>
       </c>
       <c r="D7" t="n">
-        <v>3.522029311862801e-16</v>
+        <v>2.619326660394694e-05</v>
       </c>
       <c r="E7" t="n">
-        <v>-7.30217223007195e-13</v>
+        <v>-0.02469211924328284</v>
       </c>
       <c r="F7" t="n">
-        <v>-7.30217223007195e-13</v>
+        <v>-0.02469211924328284</v>
       </c>
     </row>
     <row r="8">
@@ -1058,19 +1058,19 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.113002734661907e-12</v>
+        <v>-0.05050998333230372</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.113002734661907e-12</v>
+        <v>-0.05050998333230372</v>
       </c>
       <c r="D8" t="n">
-        <v>1.389446773564955e-15</v>
+        <v>4.31265915995253e-05</v>
       </c>
       <c r="E8" t="n">
-        <v>-1.111613287888342e-12</v>
+        <v>-0.0504668567407042</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.111613287888342e-12</v>
+        <v>-0.05046685674070419</v>
       </c>
     </row>
     <row r="9">
@@ -1078,19 +1078,19 @@
         <v>0.7000000000000001</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.617175242298278e-12</v>
+        <v>-0.09263675509813554</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.617175242298279e-12</v>
+        <v>-0.09263675509813553</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.029612907584281e-15</v>
+        <v>6.576770868279297e-05</v>
       </c>
       <c r="E9" t="n">
-        <v>-1.618204855205863e-12</v>
+        <v>-0.09257098738945276</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.618204855205863e-12</v>
+        <v>-0.09257098738945273</v>
       </c>
     </row>
     <row r="10">
@@ -1098,19 +1098,19 @@
         <v>0.8</v>
       </c>
       <c r="B10" t="n">
-        <v>-1.932843469756503e-12</v>
+        <v>-0.156834190479056</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.932843469756503e-12</v>
+        <v>-0.156834190479056</v>
       </c>
       <c r="D10" t="n">
-        <v>1.804859375020941e-15</v>
+        <v>9.524810557218265e-05</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.931038610381482e-12</v>
+        <v>-0.1567389423734838</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.931038610381482e-12</v>
+        <v>-0.1567389423734838</v>
       </c>
     </row>
     <row r="11">
@@ -1118,19 +1118,19 @@
         <v>0.9</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.062768833439539e-12</v>
+        <v>-0.2496707745683509</v>
       </c>
       <c r="C11" t="n">
-        <v>-2.062768833439539e-12</v>
+        <v>-0.2496707745683509</v>
       </c>
       <c r="D11" t="n">
-        <v>-2.151948108198197e-15</v>
+        <v>0.0001321140108289982</v>
       </c>
       <c r="E11" t="n">
-        <v>-2.064920781547738e-12</v>
+        <v>-0.2495386605575219</v>
       </c>
       <c r="F11" t="n">
-        <v>-2.064920781547738e-12</v>
+        <v>-0.2495386605575219</v>
       </c>
     </row>
     <row r="12">
@@ -1138,19 +1138,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.009963858459272e-12</v>
+        <v>-0.3785351403680159</v>
       </c>
       <c r="C12" t="n">
-        <v>-2.009963858459272e-12</v>
+        <v>-0.3785351403680159</v>
       </c>
       <c r="D12" t="n">
-        <v>2.155988146992593e-15</v>
+        <v>0.0001774117549150616</v>
       </c>
       <c r="E12" t="n">
-        <v>-2.00780787031228e-12</v>
+        <v>-0.3783577286131009</v>
       </c>
       <c r="F12" t="n">
-        <v>-2.00780787031228e-12</v>
+        <v>-0.3783577286131009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>